<commit_message>
Separated linear regression from the topic modeling run and created UI for it
</commit_message>
<xml_diff>
--- a/close_types.xlsx
+++ b/close_types.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shlomin\PycharmProjects\lda_test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724BC2AD-B3D2-4EFB-9F68-200BC9CF21C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65006127-B3AA-4AB0-9934-24264A39D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28965" yWindow="-165" windowWidth="29130" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="close_types" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Parent</t>
   </si>
@@ -91,16 +90,22 @@
     <t>Men on Males and Females</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Peer</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Male Role Model</t>
+  </si>
+  <si>
+    <t>Female Role Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,6 +422,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -578,8 +589,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -698,7 +711,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Female</c:v>
+                  <c:v>Female Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -725,7 +738,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -734,16 +747,16 @@
             <c:numRef>
               <c:f>close_types!$T$4:$V$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>57.461024498886417</c:v>
+                  <c:v>0.57461024498886415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.481069042316257</c:v>
+                  <c:v>0.16481069042316257</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.057906458797326</c:v>
+                  <c:v>0.26057906458797325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -763,7 +776,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Male</c:v>
+                  <c:v>Male Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -790,7 +803,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -799,16 +812,16 @@
             <c:numRef>
               <c:f>close_types!$T$5:$V$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>53.915662650602414</c:v>
+                  <c:v>0.53915662650602414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.204819277108431</c:v>
+                  <c:v>0.26204819277108432</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.879518072289155</c:v>
+                  <c:v>0.19879518072289157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,7 +917,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1082,7 +1095,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Female</c:v>
+                  <c:v>Female Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1109,7 +1122,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1118,16 +1131,16 @@
             <c:numRef>
               <c:f>close_types!$T$10:$V$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73.509933774834437</c:v>
+                  <c:v>0.73509933774834435</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.894039735099339</c:v>
+                  <c:v>0.15894039735099338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.596026490066226</c:v>
+                  <c:v>0.10596026490066225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1147,7 +1160,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Male</c:v>
+                  <c:v>Male Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1174,7 +1187,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1183,16 +1196,16 @@
             <c:numRef>
               <c:f>close_types!$T$11:$V$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>48.396094839609482</c:v>
+                  <c:v>0.48396094839609483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.799163179916317</c:v>
+                  <c:v>0.31799163179916318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.804741980474198</c:v>
+                  <c:v>0.19804741980474197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1288,7 +1301,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1530,13 +1543,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>57.461024498886417</c:v>
+                  <c:v>0.57461024498886415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.481069042316257</c:v>
+                  <c:v>0.16481069042316257</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.057906458797326</c:v>
+                  <c:v>0.26057906458797325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1595,13 +1608,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73.509933774834437</c:v>
+                  <c:v>0.73509933774834435</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.894039735099339</c:v>
+                  <c:v>0.15894039735099338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.596026490066226</c:v>
+                  <c:v>0.10596026490066225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,13 +1970,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>53.915662650602414</c:v>
+                  <c:v>0.53915662650602414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.204819277108431</c:v>
+                  <c:v>0.26204819277108432</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.879518072289155</c:v>
+                  <c:v>0.19879518072289157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2022,13 +2035,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>48.396094839609482</c:v>
+                  <c:v>0.48396094839609483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.799163179916317</c:v>
+                  <c:v>0.31799163179916318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.804741980474198</c:v>
+                  <c:v>0.19804741980474197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,7 +2345,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Female</c:v>
+                  <c:v>Female Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2359,7 +2372,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2368,16 +2381,16 @@
             <c:numRef>
               <c:f>close_types!$T$4:$V$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>57.461024498886417</c:v>
+                  <c:v>0.57461024498886415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.481069042316257</c:v>
+                  <c:v>0.16481069042316257</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.057906458797326</c:v>
+                  <c:v>0.26057906458797325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2397,7 +2410,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Male</c:v>
+                  <c:v>Male Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2424,7 +2437,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2433,16 +2446,16 @@
             <c:numRef>
               <c:f>close_types!$T$5:$V$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>53.915662650602414</c:v>
+                  <c:v>0.53915662650602414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.204819277108431</c:v>
+                  <c:v>0.26204819277108432</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.879518072289155</c:v>
+                  <c:v>0.19879518072289157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,7 +2551,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2741,7 +2754,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Female</c:v>
+                  <c:v>Female Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2768,7 +2781,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2777,16 +2790,16 @@
             <c:numRef>
               <c:f>close_types!$T$10:$V$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>73.509933774834437</c:v>
+                  <c:v>0.73509933774834435</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.894039735099339</c:v>
+                  <c:v>0.15894039735099338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.596026490066226</c:v>
+                  <c:v>0.10596026490066225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2806,7 +2819,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Male</c:v>
+                  <c:v>Male Role Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2833,7 +2846,7 @@
                   <c:v>Mentor</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Friend</c:v>
+                  <c:v>Peer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2842,16 +2855,16 @@
             <c:numRef>
               <c:f>close_types!$T$11:$V$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>48.396094839609482</c:v>
+                  <c:v>0.48396094839609483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.799163179916317</c:v>
+                  <c:v>0.31799163179916318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.804741980474198</c:v>
+                  <c:v>0.19804741980474197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2947,7 +2960,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3042,6 +3055,1176 @@
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Women</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>close_types!$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Female Role Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>close_types!$T$3:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mentor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Peer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>close_types!$T$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.57461024498886415</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16481069042316257</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26057906458797325</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1013-46D0-A7DF-B610A1E2A023}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>close_types!$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Male Role Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{50C995FD-989A-4872-827A-0F6AD7455BCD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1013-46D0-A7DF-B610A1E2A023}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B1C6B833-B56B-4971-8433-54529D527A57}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1013-46D0-A7DF-B610A1E2A023}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E8715B03-9BDD-4129-8196-9B7C5CA3B063}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1013-46D0-A7DF-B610A1E2A023}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>close_types!$T$3:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mentor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Peer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>close_types!$T$5:$V$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.53915662650602414</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26204819277108432</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19879518072289157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>close_types!$T$5:$V$5</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>53.9%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>26.2%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>19.9%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1013-46D0-A7DF-B610A1E2A023}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="694876800"/>
+        <c:axId val="694882704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="694876800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="694882704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="694882704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="694876800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Men</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>close_types!$S$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Female Role Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>close_types!$T$9:$V$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mentor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Peer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>close_types!$T$10:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.73509933774834435</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15894039735099338</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10596026490066225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DB88-4BE8-955E-3EEBF9B3E5E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>close_types!$S$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Male Role Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>close_types!$T$9:$V$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Family</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mentor</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Peer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>close_types!$T$11:$V$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.48396094839609483</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31799163179916318</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19804741980474197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DB88-4BE8-955E-3EEBF9B3E5E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="693799968"/>
+        <c:axId val="693798656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="693799968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="693798656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="693798656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="693799968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -3305,6 +4488,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5821,6 +7084,1012 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6541,6 +8810,87 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Group 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28ABFCDD-913E-478E-8489-6093D5A05776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7813675" y="9591675"/>
+          <a:ext cx="9144000" cy="2886075"/>
+          <a:chOff x="7807325" y="9588500"/>
+          <a:chExt cx="9144000" cy="2889250"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="8" name="Chart 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC3C50F5-61E4-4CCE-BA94-39453CFDB1D1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="7807325" y="9588500"/>
+          <a:ext cx="4572000" cy="2889250"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="9" name="Chart 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FE2A1C7-ABF8-4538-A9C1-46DE2183EE45}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="12379325" y="9588500"/>
+          <a:ext cx="4572000" cy="2889250"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6841,436 +9191,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="S2" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="S2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AA3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>611</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>174</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>41</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>27</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>24</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>50</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>117</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <f>C4+D4+F4+E4</f>
         <v>258</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <f>G4+H4</f>
         <v>74</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="1">
         <f>I4+J4</f>
         <v>117</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="1">
         <f>SUM(M4:O4)</f>
         <v>449</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" s="2">
+        <f>M4/$P4</f>
+        <v>0.57461024498886415</v>
+      </c>
+      <c r="U4" s="2">
+        <f>N4/$P4</f>
+        <v>0.16481069042316257</v>
+      </c>
+      <c r="V4" s="2">
+        <f>O4/$P4</f>
+        <v>0.26057906458797325</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>T4</f>
+        <v>0.57461024498886415</v>
+      </c>
+      <c r="AB4" s="1">
+        <f t="shared" ref="AB4:AC4" si="0">U4</f>
+        <v>0.16481069042316257</v>
+      </c>
+      <c r="AC4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26057906458797325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1144</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1">
+        <v>48</v>
+      </c>
+      <c r="I5" s="1">
+        <v>65</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" ref="M5:M7" si="1">C5+D5+F5+E5</f>
+        <v>179</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" ref="N5:N7" si="2">G5+H5</f>
+        <v>87</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" ref="O5:O7" si="3">I5+J5</f>
+        <v>66</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" ref="P5:P7" si="4">SUM(M5:O5)</f>
+        <v>332</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="2">
+        <f>M5/$P5</f>
+        <v>0.53915662650602414</v>
+      </c>
+      <c r="U5" s="2">
+        <f>N5/$P5</f>
+        <v>0.26204819277108432</v>
+      </c>
+      <c r="V5" s="2">
+        <f>O5/$P5</f>
+        <v>0.19879518072289157</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" s="1">
+        <f>T10</f>
+        <v>0.73509933774834435</v>
+      </c>
+      <c r="AB5" s="1">
+        <f t="shared" ref="AB5:AC5" si="5">U10</f>
+        <v>0.15894039735099338</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" si="5"/>
+        <v>0.10596026490066225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>89</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2943</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>177</v>
+      </c>
+      <c r="D7" s="1">
+        <v>109</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1">
+        <v>82</v>
+      </c>
+      <c r="H7" s="1">
+        <v>146</v>
+      </c>
+      <c r="I7" s="1">
+        <v>142</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="1"/>
+        <v>347</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="2"/>
+        <v>228</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="3"/>
+        <v>142</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="4"/>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="T9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T4">
-        <f>M4/$P4*100</f>
-        <v>57.461024498886417</v>
-      </c>
-      <c r="U4">
-        <f t="shared" ref="U4:V4" si="0">N4/$P4*100</f>
-        <v>16.481069042316257</v>
-      </c>
-      <c r="V4">
-        <f t="shared" si="0"/>
-        <v>26.057906458797326</v>
-      </c>
-      <c r="Z4" t="s">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="S10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="2">
+        <f>M6/$P6</f>
+        <v>0.73509933774834435</v>
+      </c>
+      <c r="U10" s="2">
+        <f>N6/$P6</f>
+        <v>0.15894039735099338</v>
+      </c>
+      <c r="V10" s="2">
+        <f>O6/$P6</f>
+        <v>0.10596026490066225</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="S11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="2">
+        <f>M7/$P7</f>
+        <v>0.48396094839609483</v>
+      </c>
+      <c r="U11" s="2">
+        <f>N7/$P7</f>
+        <v>0.31799163179916318</v>
+      </c>
+      <c r="V11" s="2">
+        <f>O7/$P7</f>
+        <v>0.19804741980474197</v>
+      </c>
+      <c r="Z11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA4">
-        <f>T4</f>
-        <v>57.461024498886417</v>
-      </c>
-      <c r="AB4">
-        <f t="shared" ref="AB4:AC4" si="1">U4</f>
-        <v>16.481069042316257</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" si="1"/>
-        <v>26.057906458797326</v>
+      <c r="AA11" s="1">
+        <f>T5</f>
+        <v>0.53915662650602414</v>
+      </c>
+      <c r="AB11" s="1">
+        <f t="shared" ref="AB11:AC11" si="6">U5</f>
+        <v>0.26204819277108432</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" si="6"/>
+        <v>0.19879518072289157</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1144</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>95</v>
-      </c>
-      <c r="D5">
-        <v>48</v>
-      </c>
-      <c r="E5">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>13</v>
-      </c>
-      <c r="G5">
-        <v>39</v>
-      </c>
-      <c r="H5">
-        <v>48</v>
-      </c>
-      <c r="I5">
-        <v>65</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5:M7" si="2">C5+D5+F5+E5</f>
-        <v>179</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ref="N5:N7" si="3">G5+H5</f>
-        <v>87</v>
-      </c>
-      <c r="O5">
-        <f t="shared" ref="O5:O7" si="4">I5+J5</f>
-        <v>66</v>
-      </c>
-      <c r="P5">
-        <f t="shared" ref="P5:P7" si="5">SUM(M5:O5)</f>
-        <v>332</v>
-      </c>
-      <c r="S5" t="s">
-        <v>20</v>
-      </c>
-      <c r="T5">
-        <f t="shared" ref="T5" si="6">M5/$P5*100</f>
-        <v>53.915662650602414</v>
-      </c>
-      <c r="U5">
-        <f t="shared" ref="U5" si="7">N5/$P5*100</f>
-        <v>26.204819277108431</v>
-      </c>
-      <c r="V5">
-        <f t="shared" ref="V5" si="8">O5/$P5*100</f>
-        <v>19.879518072289155</v>
-      </c>
-      <c r="Z5" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA5">
-        <f>T10</f>
-        <v>73.509933774834437</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" ref="AB5:AC5" si="9">U10</f>
-        <v>15.894039735099339</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="9"/>
-        <v>10.596026490066226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>89</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>73</v>
-      </c>
-      <c r="D6">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>13</v>
-      </c>
-      <c r="I6">
-        <v>14</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="2"/>
-        <v>111</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="5"/>
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2943</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>177</v>
-      </c>
-      <c r="D7">
-        <v>109</v>
-      </c>
-      <c r="E7">
-        <v>40</v>
-      </c>
-      <c r="F7">
-        <v>21</v>
-      </c>
-      <c r="G7">
-        <v>82</v>
-      </c>
-      <c r="H7">
-        <v>146</v>
-      </c>
-      <c r="I7">
-        <v>142</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>347</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="4"/>
-        <v>142</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="5"/>
-        <v>717</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="S8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="T9" t="s">
-        <v>14</v>
-      </c>
-      <c r="U9" t="s">
-        <v>12</v>
-      </c>
-      <c r="V9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="S10" t="s">
-        <v>19</v>
-      </c>
-      <c r="T10">
-        <f>M6/$P6*100</f>
-        <v>73.509933774834437</v>
-      </c>
-      <c r="U10">
-        <f>N6/$P6*100</f>
-        <v>15.894039735099339</v>
-      </c>
-      <c r="V10">
-        <f>O6/$P6*100</f>
-        <v>10.596026490066226</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="S11" t="s">
-        <v>20</v>
-      </c>
-      <c r="T11">
-        <f>M7/$P7*100</f>
-        <v>48.396094839609482</v>
-      </c>
-      <c r="U11">
-        <f>N7/$P7*100</f>
-        <v>31.799163179916317</v>
-      </c>
-      <c r="V11">
-        <f>O7/$P7*100</f>
-        <v>19.804741980474198</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA11">
-        <f>T5</f>
-        <v>53.915662650602414</v>
-      </c>
-      <c r="AB11">
-        <f t="shared" ref="AB11:AC11" si="10">U5</f>
-        <v>26.204819277108431</v>
-      </c>
-      <c r="AC11">
-        <f t="shared" si="10"/>
-        <v>19.879518072289155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="Z12" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA12">
+      <c r="AA12" s="1">
         <f>T11</f>
-        <v>48.396094839609482</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" ref="AB12:AC12" si="11">U11</f>
-        <v>31.799163179916317</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="11"/>
-        <v>19.804741980474198</v>
+        <v>0.48396094839609483</v>
+      </c>
+      <c r="AB12" s="1">
+        <f t="shared" ref="AB12:AC12" si="7">U11</f>
+        <v>0.31799163179916318</v>
+      </c>
+      <c r="AC12" s="1">
+        <f t="shared" si="7"/>
+        <v>0.19804741980474197</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>